<commit_message>
started testing for distribution (pyinstaller) and reasonable GUI (pyQT and QT designer)
</commit_message>
<xml_diff>
--- a/tmp/klassen/2015_HS_6x/pruefungen/pruefungen.xlsx
+++ b/tmp/klassen/2015_HS_6x/pruefungen/pruefungen.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
could work out tabs in main window. new frontend in frontend (gui folder deprecated, only keeping it for reference)
</commit_message>
<xml_diff>
--- a/tmp/klassen/2015_HS_6x/pruefungen/pruefungen.xlsx
+++ b/tmp/klassen/2015_HS_6x/pruefungen/pruefungen.xlsx
@@ -825,54 +825,22 @@
           <t>marlene</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>7</v>
-      </c>
-      <c r="D11" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E11" t="n">
-        <v>21</v>
-      </c>
-      <c r="F11" t="n">
-        <v>5.7727</v>
-      </c>
-      <c r="G11" t="n">
-        <v>16</v>
-      </c>
-      <c r="H11" t="n">
-        <v>4.4783</v>
-      </c>
-      <c r="I11" t="n">
-        <v>12</v>
-      </c>
-      <c r="J11" t="n">
-        <v>5</v>
-      </c>
-      <c r="K11" t="n">
-        <v>14</v>
-      </c>
-      <c r="L11" t="n">
-        <v>5.6667</v>
-      </c>
-      <c r="M11" t="n">
-        <v>14</v>
-      </c>
-      <c r="N11" t="n">
-        <v>5.6667</v>
-      </c>
-      <c r="O11" t="n">
-        <v>28</v>
-      </c>
-      <c r="P11" t="n">
-        <v>5.6667</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>29</v>
-      </c>
-      <c r="R11" t="n">
-        <v>6</v>
-      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -885,54 +853,22 @@
           <t>alina</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>1</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>1</v>
-      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -945,54 +881,22 @@
           <t>nina</t>
         </is>
       </c>
-      <c r="C13" t="n">
-        <v>10</v>
-      </c>
-      <c r="D13" t="n">
-        <v>6</v>
-      </c>
-      <c r="E13" t="n">
-        <v>20</v>
-      </c>
-      <c r="F13" t="n">
-        <v>5.5455</v>
-      </c>
-      <c r="G13" t="n">
-        <v>15</v>
-      </c>
-      <c r="H13" t="n">
-        <v>4.2609</v>
-      </c>
-      <c r="I13" t="n">
-        <v>12</v>
-      </c>
-      <c r="J13" t="n">
-        <v>5</v>
-      </c>
-      <c r="K13" t="n">
-        <v>13</v>
-      </c>
-      <c r="L13" t="n">
-        <v>5.3333</v>
-      </c>
-      <c r="M13" t="n">
-        <v>11</v>
-      </c>
-      <c r="N13" t="n">
-        <v>4.6667</v>
-      </c>
-      <c r="O13" t="n">
-        <v>26</v>
-      </c>
-      <c r="P13" t="n">
-        <v>5.3333</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>26</v>
-      </c>
-      <c r="R13" t="n">
-        <v>5.6429</v>
-      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1005,54 +909,22 @@
           <t>noe</t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>10</v>
-      </c>
-      <c r="D14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E14" t="n">
-        <v>25</v>
-      </c>
-      <c r="F14" t="n">
-        <v>6</v>
-      </c>
-      <c r="G14" t="n">
-        <v>25</v>
-      </c>
-      <c r="H14" t="n">
-        <v>6</v>
-      </c>
-      <c r="I14" t="n">
-        <v>15</v>
-      </c>
-      <c r="J14" t="n">
-        <v>6</v>
-      </c>
-      <c r="K14" t="n">
-        <v>15</v>
-      </c>
-      <c r="L14" t="n">
-        <v>6</v>
-      </c>
-      <c r="M14" t="n">
-        <v>15</v>
-      </c>
-      <c r="N14" t="n">
-        <v>6</v>
-      </c>
-      <c r="O14" t="n">
-        <v>35</v>
-      </c>
-      <c r="P14" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>35</v>
-      </c>
-      <c r="R14" t="n">
-        <v>6</v>
-      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1065,54 +937,22 @@
           <t>nina</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>10</v>
-      </c>
-      <c r="D15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E15" t="n">
-        <v>23</v>
-      </c>
-      <c r="F15" t="n">
-        <v>6</v>
-      </c>
-      <c r="G15" t="n">
-        <v>18</v>
-      </c>
-      <c r="H15" t="n">
-        <v>4.913</v>
-      </c>
-      <c r="I15" t="n">
-        <v>14</v>
-      </c>
-      <c r="J15" t="n">
-        <v>5.6667</v>
-      </c>
-      <c r="K15" t="n">
-        <v>15</v>
-      </c>
-      <c r="L15" t="n">
-        <v>6</v>
-      </c>
-      <c r="M15" t="n">
-        <v>14</v>
-      </c>
-      <c r="N15" t="n">
-        <v>5.6667</v>
-      </c>
-      <c r="O15" t="n">
-        <v>30</v>
-      </c>
-      <c r="P15" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>29</v>
-      </c>
-      <c r="R15" t="n">
-        <v>6</v>
-      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1125,54 +965,22 @@
           <t>dominik</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>10</v>
-      </c>
-      <c r="D16" t="n">
-        <v>6</v>
-      </c>
-      <c r="E16" t="n">
-        <v>8</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2.8182</v>
-      </c>
-      <c r="G16" t="n">
-        <v>22</v>
-      </c>
-      <c r="H16" t="n">
-        <v>5.7826</v>
-      </c>
-      <c r="I16" t="n">
-        <v>15</v>
-      </c>
-      <c r="J16" t="n">
-        <v>6</v>
-      </c>
-      <c r="K16" t="n">
-        <v>7</v>
-      </c>
-      <c r="L16" t="n">
-        <v>3.3333</v>
-      </c>
-      <c r="M16" t="n">
-        <v>9</v>
-      </c>
-      <c r="N16" t="n">
-        <v>4</v>
-      </c>
-      <c r="O16" t="n">
-        <v>17</v>
-      </c>
-      <c r="P16" t="n">
-        <v>3.8333</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>17</v>
-      </c>
-      <c r="R16" t="n">
-        <v>4.0357</v>
-      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1185,54 +993,22 @@
           <t>nicolas</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>10</v>
-      </c>
-      <c r="D17" t="n">
-        <v>6</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" t="n">
-        <v>23</v>
-      </c>
-      <c r="H17" t="n">
-        <v>6</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17" t="n">
-        <v>15</v>
-      </c>
-      <c r="L17" t="n">
-        <v>6</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>25</v>
-      </c>
-      <c r="R17" t="n">
-        <v>5.4643</v>
-      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>